<commit_message>
exam code , created date feature update by ganga
</commit_message>
<xml_diff>
--- a/ExamPortal/backend/backend_dotnet/Examportal/Files/javascriptQuiz.xlsx
+++ b/ExamPortal/backend/backend_dotnet/Examportal/Files/javascriptQuiz.xlsx
@@ -642,163 +642,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100272AC0B6D109A84FA89166B7C73D4528" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ebcfe8fb11b33402d3a4b2c7dcfa0cd3">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8672fc5b-9772-44e9-b4a2-d27b44082db3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a45e58237d3cf8679d8d3a8cefb282bd" ns2:_="">
-    <xsd:import namespace="8672fc5b-9772-44e9-b4a2-d27b44082db3"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="8672fc5b-9772-44e9-b4a2-d27b44082db3" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DFC6167-1AC6-4B45-B9D3-619797D7561A}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{955D7B4F-E8CC-4FEE-AFDC-6CDE67BFEBA1}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24253F4E-BAC8-4D08-B1CD-B542FC10DD1D}"/>
 </file>
</xml_diff>

<commit_message>
bugs related to test fixed
</commit_message>
<xml_diff>
--- a/ExamPortal/backend/backend_dotnet/Examportal/Files/javascriptQuiz.xlsx
+++ b/ExamPortal/backend/backend_dotnet/Examportal/Files/javascriptQuiz.xlsx
@@ -642,4 +642,163 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100272AC0B6D109A84FA89166B7C73D4528" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ebcfe8fb11b33402d3a4b2c7dcfa0cd3">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8672fc5b-9772-44e9-b4a2-d27b44082db3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a45e58237d3cf8679d8d3a8cefb282bd" ns2:_="">
+    <xsd:import namespace="8672fc5b-9772-44e9-b4a2-d27b44082db3"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="8672fc5b-9772-44e9-b4a2-d27b44082db3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DFC6167-1AC6-4B45-B9D3-619797D7561A}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{955D7B4F-E8CC-4FEE-AFDC-6CDE67BFEBA1}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24253F4E-BAC8-4D08-B1CD-B542FC10DD1D}"/>
 </file>
</xml_diff>

<commit_message>
question upload with image done and question update also done, delete exam and question issue also fixed
</commit_message>
<xml_diff>
--- a/ExamPortal/backend/backend_dotnet/Examportal/Files/javascriptQuiz.xlsx
+++ b/ExamPortal/backend/backend_dotnet/Examportal/Files/javascriptQuiz.xlsx
@@ -642,4 +642,163 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100272AC0B6D109A84FA89166B7C73D4528" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ebcfe8fb11b33402d3a4b2c7dcfa0cd3">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8672fc5b-9772-44e9-b4a2-d27b44082db3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a45e58237d3cf8679d8d3a8cefb282bd" ns2:_="">
+    <xsd:import namespace="8672fc5b-9772-44e9-b4a2-d27b44082db3"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="8672fc5b-9772-44e9-b4a2-d27b44082db3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DFC6167-1AC6-4B45-B9D3-619797D7561A}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{955D7B4F-E8CC-4FEE-AFDC-6CDE67BFEBA1}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24253F4E-BAC8-4D08-B1CD-B542FC10DD1D}"/>
 </file>
</xml_diff>

<commit_message>
student performance controller created
</commit_message>
<xml_diff>
--- a/ExamPortal/backend/backend_dotnet/Examportal/Files/javascriptQuiz.xlsx
+++ b/ExamPortal/backend/backend_dotnet/Examportal/Files/javascriptQuiz.xlsx
@@ -642,4 +642,163 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100272AC0B6D109A84FA89166B7C73D4528" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ebcfe8fb11b33402d3a4b2c7dcfa0cd3">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8672fc5b-9772-44e9-b4a2-d27b44082db3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a45e58237d3cf8679d8d3a8cefb282bd" ns2:_="">
+    <xsd:import namespace="8672fc5b-9772-44e9-b4a2-d27b44082db3"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="8672fc5b-9772-44e9-b4a2-d27b44082db3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DFC6167-1AC6-4B45-B9D3-619797D7561A}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{955D7B4F-E8CC-4FEE-AFDC-6CDE67BFEBA1}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24253F4E-BAC8-4D08-B1CD-B542FC10DD1D}"/>
 </file>
</xml_diff>